<commit_message>
fix channel (CHW to HWC) in keras
</commit_message>
<xml_diff>
--- a/outputs/tf/ResNet50.xlsx
+++ b/outputs/tf/ResNet50.xlsx
@@ -610,47 +610,47 @@
       </c>
       <c r="D2" s="10" t="inlineStr">
         <is>
+          <t>Height</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="inlineStr">
+        <is>
+          <t>Width</t>
+        </is>
+      </c>
+      <c r="F2" s="10" t="inlineStr">
+        <is>
           <t>Channel</t>
         </is>
       </c>
-      <c r="E2" s="10" t="inlineStr">
+      <c r="G2" s="10" t="inlineStr">
         <is>
           <t>Height</t>
         </is>
       </c>
-      <c r="F2" s="10" t="inlineStr">
+      <c r="H2" s="10" t="inlineStr">
         <is>
           <t>Width</t>
         </is>
       </c>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="I2" s="10" t="inlineStr">
         <is>
           <t>Channel</t>
         </is>
       </c>
-      <c r="H2" s="10" t="inlineStr">
+      <c r="J2" s="10" t="inlineStr">
         <is>
           <t>Height</t>
         </is>
       </c>
-      <c r="I2" s="10" t="inlineStr">
+      <c r="K2" s="10" t="inlineStr">
         <is>
           <t>Width</t>
         </is>
       </c>
-      <c r="J2" s="10" t="inlineStr">
+      <c r="L2" s="10" t="inlineStr">
         <is>
           <t>Channel</t>
-        </is>
-      </c>
-      <c r="K2" s="10" t="inlineStr">
-        <is>
-          <t>Height</t>
-        </is>
-      </c>
-      <c r="L2" s="10" t="inlineStr">
-        <is>
-          <t>Width</t>
         </is>
       </c>
       <c r="M2" s="10" t="inlineStr">

</xml_diff>

<commit_message>
update keras part to match pytorch, backops added
</commit_message>
<xml_diff>
--- a/outputs/tf/ResNet50.xlsx
+++ b/outputs/tf/ResNet50.xlsx
@@ -906,7 +906,9 @@
       </c>
       <c r="W5" s="8" t="n"/>
       <c r="X5" s="8" t="n"/>
-      <c r="Y5" s="8" t="n"/>
+      <c r="Y5" s="8" t="n">
+        <v>118014016</v>
+      </c>
       <c r="Z5" s="8" t="n"/>
       <c r="AA5" s="8" t="n"/>
     </row>
@@ -966,7 +968,9 @@
       </c>
       <c r="X6" s="8" t="n"/>
       <c r="Y6" s="8" t="n"/>
-      <c r="Z6" s="8" t="n"/>
+      <c r="Z6" s="8" t="n">
+        <v>1605632</v>
+      </c>
       <c r="AA6" s="8" t="n"/>
     </row>
     <row r="7">
@@ -1024,7 +1028,9 @@
       </c>
       <c r="Y7" s="8" t="n"/>
       <c r="Z7" s="8" t="n"/>
-      <c r="AA7" s="8" t="n"/>
+      <c r="AA7" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="n">
@@ -1147,7 +1153,9 @@
       </c>
       <c r="X9" s="8" t="n"/>
       <c r="Y9" s="8" t="n"/>
-      <c r="Z9" s="8" t="n"/>
+      <c r="Z9" s="8" t="n">
+        <v>1806336</v>
+      </c>
       <c r="AA9" s="8" t="n"/>
     </row>
     <row r="10">
@@ -1217,7 +1225,9 @@
       </c>
       <c r="W10" s="8" t="n"/>
       <c r="X10" s="8" t="n"/>
-      <c r="Y10" s="8" t="n"/>
+      <c r="Y10" s="8" t="n">
+        <v>12845120</v>
+      </c>
       <c r="Z10" s="8" t="n"/>
       <c r="AA10" s="8" t="n"/>
     </row>
@@ -1277,7 +1287,9 @@
       </c>
       <c r="X11" s="8" t="n"/>
       <c r="Y11" s="8" t="n"/>
-      <c r="Z11" s="8" t="n"/>
+      <c r="Z11" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA11" s="8" t="n"/>
     </row>
     <row r="12">
@@ -1335,7 +1347,9 @@
       </c>
       <c r="Y12" s="8" t="n"/>
       <c r="Z12" s="8" t="n"/>
-      <c r="AA12" s="8" t="n"/>
+      <c r="AA12" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="7" t="n">
@@ -1404,7 +1418,9 @@
       </c>
       <c r="W13" s="8" t="n"/>
       <c r="X13" s="8" t="n"/>
-      <c r="Y13" s="8" t="n"/>
+      <c r="Y13" s="8" t="n">
+        <v>115605568</v>
+      </c>
       <c r="Z13" s="8" t="n"/>
       <c r="AA13" s="8" t="n"/>
     </row>
@@ -1464,7 +1480,9 @@
       </c>
       <c r="X14" s="8" t="n"/>
       <c r="Y14" s="8" t="n"/>
-      <c r="Z14" s="8" t="n"/>
+      <c r="Z14" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA14" s="8" t="n"/>
     </row>
     <row r="15">
@@ -1522,7 +1540,9 @@
       </c>
       <c r="Y15" s="8" t="n"/>
       <c r="Z15" s="8" t="n"/>
-      <c r="AA15" s="8" t="n"/>
+      <c r="AA15" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="7" t="n">
@@ -1591,7 +1611,9 @@
       </c>
       <c r="W16" s="8" t="n"/>
       <c r="X16" s="8" t="n"/>
-      <c r="Y16" s="8" t="n"/>
+      <c r="Y16" s="8" t="n">
+        <v>51380480</v>
+      </c>
       <c r="Z16" s="8" t="n"/>
       <c r="AA16" s="8" t="n"/>
     </row>
@@ -1662,7 +1684,9 @@
       </c>
       <c r="W17" s="8" t="n"/>
       <c r="X17" s="8" t="n"/>
-      <c r="Y17" s="8" t="n"/>
+      <c r="Y17" s="8" t="n">
+        <v>51380480</v>
+      </c>
       <c r="Z17" s="8" t="n"/>
       <c r="AA17" s="8" t="n"/>
     </row>
@@ -1722,7 +1746,9 @@
       </c>
       <c r="X18" s="8" t="n"/>
       <c r="Y18" s="8" t="n"/>
-      <c r="Z18" s="8" t="n"/>
+      <c r="Z18" s="8" t="n">
+        <v>1605632</v>
+      </c>
       <c r="AA18" s="8" t="n"/>
     </row>
     <row r="19">
@@ -1781,7 +1807,9 @@
       </c>
       <c r="X19" s="8" t="n"/>
       <c r="Y19" s="8" t="n"/>
-      <c r="Z19" s="8" t="n"/>
+      <c r="Z19" s="8" t="n">
+        <v>1605632</v>
+      </c>
       <c r="AA19" s="8" t="n"/>
     </row>
     <row r="20">
@@ -1844,7 +1872,9 @@
       </c>
       <c r="X20" s="8" t="n"/>
       <c r="Y20" s="8" t="n"/>
-      <c r="Z20" s="8" t="n"/>
+      <c r="Z20" s="8" t="n">
+        <v>802816</v>
+      </c>
       <c r="AA20" s="8" t="n"/>
     </row>
     <row r="21">
@@ -1902,7 +1932,9 @@
       </c>
       <c r="Y21" s="8" t="n"/>
       <c r="Z21" s="8" t="n"/>
-      <c r="AA21" s="8" t="n"/>
+      <c r="AA21" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n">
@@ -1971,7 +2003,9 @@
       </c>
       <c r="W22" s="8" t="n"/>
       <c r="X22" s="8" t="n"/>
-      <c r="Y22" s="8" t="n"/>
+      <c r="Y22" s="8" t="n">
+        <v>51380288</v>
+      </c>
       <c r="Z22" s="8" t="n"/>
       <c r="AA22" s="8" t="n"/>
     </row>
@@ -2031,7 +2065,9 @@
       </c>
       <c r="X23" s="8" t="n"/>
       <c r="Y23" s="8" t="n"/>
-      <c r="Z23" s="8" t="n"/>
+      <c r="Z23" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA23" s="8" t="n"/>
     </row>
     <row r="24">
@@ -2089,7 +2125,9 @@
       </c>
       <c r="Y24" s="8" t="n"/>
       <c r="Z24" s="8" t="n"/>
-      <c r="AA24" s="8" t="n"/>
+      <c r="AA24" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="n">
@@ -2158,7 +2196,9 @@
       </c>
       <c r="W25" s="8" t="n"/>
       <c r="X25" s="8" t="n"/>
-      <c r="Y25" s="8" t="n"/>
+      <c r="Y25" s="8" t="n">
+        <v>115605568</v>
+      </c>
       <c r="Z25" s="8" t="n"/>
       <c r="AA25" s="8" t="n"/>
     </row>
@@ -2218,7 +2258,9 @@
       </c>
       <c r="X26" s="8" t="n"/>
       <c r="Y26" s="8" t="n"/>
-      <c r="Z26" s="8" t="n"/>
+      <c r="Z26" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA26" s="8" t="n"/>
     </row>
     <row r="27">
@@ -2276,7 +2318,9 @@
       </c>
       <c r="Y27" s="8" t="n"/>
       <c r="Z27" s="8" t="n"/>
-      <c r="AA27" s="8" t="n"/>
+      <c r="AA27" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="7" t="n">
@@ -2345,7 +2389,9 @@
       </c>
       <c r="W28" s="8" t="n"/>
       <c r="X28" s="8" t="n"/>
-      <c r="Y28" s="8" t="n"/>
+      <c r="Y28" s="8" t="n">
+        <v>51380480</v>
+      </c>
       <c r="Z28" s="8" t="n"/>
       <c r="AA28" s="8" t="n"/>
     </row>
@@ -2405,7 +2451,9 @@
       </c>
       <c r="X29" s="8" t="n"/>
       <c r="Y29" s="8" t="n"/>
-      <c r="Z29" s="8" t="n"/>
+      <c r="Z29" s="8" t="n">
+        <v>1605632</v>
+      </c>
       <c r="AA29" s="8" t="n"/>
     </row>
     <row r="30">
@@ -2468,7 +2516,9 @@
       </c>
       <c r="X30" s="8" t="n"/>
       <c r="Y30" s="8" t="n"/>
-      <c r="Z30" s="8" t="n"/>
+      <c r="Z30" s="8" t="n">
+        <v>802816</v>
+      </c>
       <c r="AA30" s="8" t="n"/>
     </row>
     <row r="31">
@@ -2526,7 +2576,9 @@
       </c>
       <c r="Y31" s="8" t="n"/>
       <c r="Z31" s="8" t="n"/>
-      <c r="AA31" s="8" t="n"/>
+      <c r="AA31" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="7" t="n">
@@ -2595,7 +2647,9 @@
       </c>
       <c r="W32" s="8" t="n"/>
       <c r="X32" s="8" t="n"/>
-      <c r="Y32" s="8" t="n"/>
+      <c r="Y32" s="8" t="n">
+        <v>51380288</v>
+      </c>
       <c r="Z32" s="8" t="n"/>
       <c r="AA32" s="8" t="n"/>
     </row>
@@ -2655,7 +2709,9 @@
       </c>
       <c r="X33" s="8" t="n"/>
       <c r="Y33" s="8" t="n"/>
-      <c r="Z33" s="8" t="n"/>
+      <c r="Z33" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA33" s="8" t="n"/>
     </row>
     <row r="34">
@@ -2713,7 +2769,9 @@
       </c>
       <c r="Y34" s="8" t="n"/>
       <c r="Z34" s="8" t="n"/>
-      <c r="AA34" s="8" t="n"/>
+      <c r="AA34" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="7" t="n">
@@ -2782,7 +2840,9 @@
       </c>
       <c r="W35" s="8" t="n"/>
       <c r="X35" s="8" t="n"/>
-      <c r="Y35" s="8" t="n"/>
+      <c r="Y35" s="8" t="n">
+        <v>115605568</v>
+      </c>
       <c r="Z35" s="8" t="n"/>
       <c r="AA35" s="8" t="n"/>
     </row>
@@ -2842,7 +2902,9 @@
       </c>
       <c r="X36" s="8" t="n"/>
       <c r="Y36" s="8" t="n"/>
-      <c r="Z36" s="8" t="n"/>
+      <c r="Z36" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA36" s="8" t="n"/>
     </row>
     <row r="37">
@@ -2900,7 +2962,9 @@
       </c>
       <c r="Y37" s="8" t="n"/>
       <c r="Z37" s="8" t="n"/>
-      <c r="AA37" s="8" t="n"/>
+      <c r="AA37" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="7" t="n">
@@ -2969,7 +3033,9 @@
       </c>
       <c r="W38" s="8" t="n"/>
       <c r="X38" s="8" t="n"/>
-      <c r="Y38" s="8" t="n"/>
+      <c r="Y38" s="8" t="n">
+        <v>51380480</v>
+      </c>
       <c r="Z38" s="8" t="n"/>
       <c r="AA38" s="8" t="n"/>
     </row>
@@ -3029,7 +3095,9 @@
       </c>
       <c r="X39" s="8" t="n"/>
       <c r="Y39" s="8" t="n"/>
-      <c r="Z39" s="8" t="n"/>
+      <c r="Z39" s="8" t="n">
+        <v>1605632</v>
+      </c>
       <c r="AA39" s="8" t="n"/>
     </row>
     <row r="40">
@@ -3092,7 +3160,9 @@
       </c>
       <c r="X40" s="8" t="n"/>
       <c r="Y40" s="8" t="n"/>
-      <c r="Z40" s="8" t="n"/>
+      <c r="Z40" s="8" t="n">
+        <v>802816</v>
+      </c>
       <c r="AA40" s="8" t="n"/>
     </row>
     <row r="41">
@@ -3150,7 +3220,9 @@
       </c>
       <c r="Y41" s="8" t="n"/>
       <c r="Z41" s="8" t="n"/>
-      <c r="AA41" s="8" t="n"/>
+      <c r="AA41" s="8" t="n">
+        <v>802816</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="7" t="n">
@@ -3219,7 +3291,9 @@
       </c>
       <c r="W42" s="8" t="n"/>
       <c r="X42" s="8" t="n"/>
-      <c r="Y42" s="8" t="n"/>
+      <c r="Y42" s="8" t="n">
+        <v>25690240</v>
+      </c>
       <c r="Z42" s="8" t="n"/>
       <c r="AA42" s="8" t="n"/>
     </row>
@@ -3279,7 +3353,9 @@
       </c>
       <c r="X43" s="8" t="n"/>
       <c r="Y43" s="8" t="n"/>
-      <c r="Z43" s="8" t="n"/>
+      <c r="Z43" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA43" s="8" t="n"/>
     </row>
     <row r="44">
@@ -3337,7 +3413,9 @@
       </c>
       <c r="Y44" s="8" t="n"/>
       <c r="Z44" s="8" t="n"/>
-      <c r="AA44" s="8" t="n"/>
+      <c r="AA44" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="n">
@@ -3406,7 +3484,9 @@
       </c>
       <c r="W45" s="8" t="n"/>
       <c r="X45" s="8" t="n"/>
-      <c r="Y45" s="8" t="n"/>
+      <c r="Y45" s="8" t="n">
+        <v>115605632</v>
+      </c>
       <c r="Z45" s="8" t="n"/>
       <c r="AA45" s="8" t="n"/>
     </row>
@@ -3466,7 +3546,9 @@
       </c>
       <c r="X46" s="8" t="n"/>
       <c r="Y46" s="8" t="n"/>
-      <c r="Z46" s="8" t="n"/>
+      <c r="Z46" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA46" s="8" t="n"/>
     </row>
     <row r="47">
@@ -3524,7 +3606,9 @@
       </c>
       <c r="Y47" s="8" t="n"/>
       <c r="Z47" s="8" t="n"/>
-      <c r="AA47" s="8" t="n"/>
+      <c r="AA47" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="7" t="n">
@@ -3593,7 +3677,9 @@
       </c>
       <c r="W48" s="8" t="n"/>
       <c r="X48" s="8" t="n"/>
-      <c r="Y48" s="8" t="n"/>
+      <c r="Y48" s="8" t="n">
+        <v>102760960</v>
+      </c>
       <c r="Z48" s="8" t="n"/>
       <c r="AA48" s="8" t="n"/>
     </row>
@@ -3664,7 +3750,9 @@
       </c>
       <c r="W49" s="8" t="n"/>
       <c r="X49" s="8" t="n"/>
-      <c r="Y49" s="8" t="n"/>
+      <c r="Y49" s="8" t="n">
+        <v>51380736</v>
+      </c>
       <c r="Z49" s="8" t="n"/>
       <c r="AA49" s="8" t="n"/>
     </row>
@@ -3724,7 +3812,9 @@
       </c>
       <c r="X50" s="8" t="n"/>
       <c r="Y50" s="8" t="n"/>
-      <c r="Z50" s="8" t="n"/>
+      <c r="Z50" s="8" t="n">
+        <v>802816</v>
+      </c>
       <c r="AA50" s="8" t="n"/>
     </row>
     <row r="51">
@@ -3783,7 +3873,9 @@
       </c>
       <c r="X51" s="8" t="n"/>
       <c r="Y51" s="8" t="n"/>
-      <c r="Z51" s="8" t="n"/>
+      <c r="Z51" s="8" t="n">
+        <v>802816</v>
+      </c>
       <c r="AA51" s="8" t="n"/>
     </row>
     <row r="52">
@@ -3846,7 +3938,9 @@
       </c>
       <c r="X52" s="8" t="n"/>
       <c r="Y52" s="8" t="n"/>
-      <c r="Z52" s="8" t="n"/>
+      <c r="Z52" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA52" s="8" t="n"/>
     </row>
     <row r="53">
@@ -3904,7 +3998,9 @@
       </c>
       <c r="Y53" s="8" t="n"/>
       <c r="Z53" s="8" t="n"/>
-      <c r="AA53" s="8" t="n"/>
+      <c r="AA53" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="7" t="n">
@@ -3973,7 +4069,9 @@
       </c>
       <c r="W54" s="8" t="n"/>
       <c r="X54" s="8" t="n"/>
-      <c r="Y54" s="8" t="n"/>
+      <c r="Y54" s="8" t="n">
+        <v>51380352</v>
+      </c>
       <c r="Z54" s="8" t="n"/>
       <c r="AA54" s="8" t="n"/>
     </row>
@@ -4033,7 +4131,9 @@
       </c>
       <c r="X55" s="8" t="n"/>
       <c r="Y55" s="8" t="n"/>
-      <c r="Z55" s="8" t="n"/>
+      <c r="Z55" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA55" s="8" t="n"/>
     </row>
     <row r="56">
@@ -4091,7 +4191,9 @@
       </c>
       <c r="Y56" s="8" t="n"/>
       <c r="Z56" s="8" t="n"/>
-      <c r="AA56" s="8" t="n"/>
+      <c r="AA56" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="7" t="n">
@@ -4160,7 +4262,9 @@
       </c>
       <c r="W57" s="8" t="n"/>
       <c r="X57" s="8" t="n"/>
-      <c r="Y57" s="8" t="n"/>
+      <c r="Y57" s="8" t="n">
+        <v>115605632</v>
+      </c>
       <c r="Z57" s="8" t="n"/>
       <c r="AA57" s="8" t="n"/>
     </row>
@@ -4220,7 +4324,9 @@
       </c>
       <c r="X58" s="8" t="n"/>
       <c r="Y58" s="8" t="n"/>
-      <c r="Z58" s="8" t="n"/>
+      <c r="Z58" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA58" s="8" t="n"/>
     </row>
     <row r="59">
@@ -4278,7 +4384,9 @@
       </c>
       <c r="Y59" s="8" t="n"/>
       <c r="Z59" s="8" t="n"/>
-      <c r="AA59" s="8" t="n"/>
+      <c r="AA59" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="7" t="n">
@@ -4347,7 +4455,9 @@
       </c>
       <c r="W60" s="8" t="n"/>
       <c r="X60" s="8" t="n"/>
-      <c r="Y60" s="8" t="n"/>
+      <c r="Y60" s="8" t="n">
+        <v>51380736</v>
+      </c>
       <c r="Z60" s="8" t="n"/>
       <c r="AA60" s="8" t="n"/>
     </row>
@@ -4407,7 +4517,9 @@
       </c>
       <c r="X61" s="8" t="n"/>
       <c r="Y61" s="8" t="n"/>
-      <c r="Z61" s="8" t="n"/>
+      <c r="Z61" s="8" t="n">
+        <v>802816</v>
+      </c>
       <c r="AA61" s="8" t="n"/>
     </row>
     <row r="62">
@@ -4470,7 +4582,9 @@
       </c>
       <c r="X62" s="8" t="n"/>
       <c r="Y62" s="8" t="n"/>
-      <c r="Z62" s="8" t="n"/>
+      <c r="Z62" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA62" s="8" t="n"/>
     </row>
     <row r="63">
@@ -4528,7 +4642,9 @@
       </c>
       <c r="Y63" s="8" t="n"/>
       <c r="Z63" s="8" t="n"/>
-      <c r="AA63" s="8" t="n"/>
+      <c r="AA63" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="7" t="n">
@@ -4597,7 +4713,9 @@
       </c>
       <c r="W64" s="8" t="n"/>
       <c r="X64" s="8" t="n"/>
-      <c r="Y64" s="8" t="n"/>
+      <c r="Y64" s="8" t="n">
+        <v>51380352</v>
+      </c>
       <c r="Z64" s="8" t="n"/>
       <c r="AA64" s="8" t="n"/>
     </row>
@@ -4657,7 +4775,9 @@
       </c>
       <c r="X65" s="8" t="n"/>
       <c r="Y65" s="8" t="n"/>
-      <c r="Z65" s="8" t="n"/>
+      <c r="Z65" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA65" s="8" t="n"/>
     </row>
     <row r="66">
@@ -4715,7 +4835,9 @@
       </c>
       <c r="Y66" s="8" t="n"/>
       <c r="Z66" s="8" t="n"/>
-      <c r="AA66" s="8" t="n"/>
+      <c r="AA66" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="7" t="n">
@@ -4784,7 +4906,9 @@
       </c>
       <c r="W67" s="8" t="n"/>
       <c r="X67" s="8" t="n"/>
-      <c r="Y67" s="8" t="n"/>
+      <c r="Y67" s="8" t="n">
+        <v>115605632</v>
+      </c>
       <c r="Z67" s="8" t="n"/>
       <c r="AA67" s="8" t="n"/>
     </row>
@@ -4844,7 +4968,9 @@
       </c>
       <c r="X68" s="8" t="n"/>
       <c r="Y68" s="8" t="n"/>
-      <c r="Z68" s="8" t="n"/>
+      <c r="Z68" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA68" s="8" t="n"/>
     </row>
     <row r="69">
@@ -4902,7 +5028,9 @@
       </c>
       <c r="Y69" s="8" t="n"/>
       <c r="Z69" s="8" t="n"/>
-      <c r="AA69" s="8" t="n"/>
+      <c r="AA69" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="7" t="n">
@@ -4971,7 +5099,9 @@
       </c>
       <c r="W70" s="8" t="n"/>
       <c r="X70" s="8" t="n"/>
-      <c r="Y70" s="8" t="n"/>
+      <c r="Y70" s="8" t="n">
+        <v>51380736</v>
+      </c>
       <c r="Z70" s="8" t="n"/>
       <c r="AA70" s="8" t="n"/>
     </row>
@@ -5031,7 +5161,9 @@
       </c>
       <c r="X71" s="8" t="n"/>
       <c r="Y71" s="8" t="n"/>
-      <c r="Z71" s="8" t="n"/>
+      <c r="Z71" s="8" t="n">
+        <v>802816</v>
+      </c>
       <c r="AA71" s="8" t="n"/>
     </row>
     <row r="72">
@@ -5094,7 +5226,9 @@
       </c>
       <c r="X72" s="8" t="n"/>
       <c r="Y72" s="8" t="n"/>
-      <c r="Z72" s="8" t="n"/>
+      <c r="Z72" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA72" s="8" t="n"/>
     </row>
     <row r="73">
@@ -5152,7 +5286,9 @@
       </c>
       <c r="Y73" s="8" t="n"/>
       <c r="Z73" s="8" t="n"/>
-      <c r="AA73" s="8" t="n"/>
+      <c r="AA73" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="7" t="n">
@@ -5221,7 +5357,9 @@
       </c>
       <c r="W74" s="8" t="n"/>
       <c r="X74" s="8" t="n"/>
-      <c r="Y74" s="8" t="n"/>
+      <c r="Y74" s="8" t="n">
+        <v>51380352</v>
+      </c>
       <c r="Z74" s="8" t="n"/>
       <c r="AA74" s="8" t="n"/>
     </row>
@@ -5281,7 +5419,9 @@
       </c>
       <c r="X75" s="8" t="n"/>
       <c r="Y75" s="8" t="n"/>
-      <c r="Z75" s="8" t="n"/>
+      <c r="Z75" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA75" s="8" t="n"/>
     </row>
     <row r="76">
@@ -5339,7 +5479,9 @@
       </c>
       <c r="Y76" s="8" t="n"/>
       <c r="Z76" s="8" t="n"/>
-      <c r="AA76" s="8" t="n"/>
+      <c r="AA76" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="7" t="n">
@@ -5408,7 +5550,9 @@
       </c>
       <c r="W77" s="8" t="n"/>
       <c r="X77" s="8" t="n"/>
-      <c r="Y77" s="8" t="n"/>
+      <c r="Y77" s="8" t="n">
+        <v>115605632</v>
+      </c>
       <c r="Z77" s="8" t="n"/>
       <c r="AA77" s="8" t="n"/>
     </row>
@@ -5468,7 +5612,9 @@
       </c>
       <c r="X78" s="8" t="n"/>
       <c r="Y78" s="8" t="n"/>
-      <c r="Z78" s="8" t="n"/>
+      <c r="Z78" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA78" s="8" t="n"/>
     </row>
     <row r="79">
@@ -5526,7 +5672,9 @@
       </c>
       <c r="Y79" s="8" t="n"/>
       <c r="Z79" s="8" t="n"/>
-      <c r="AA79" s="8" t="n"/>
+      <c r="AA79" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="7" t="n">
@@ -5595,7 +5743,9 @@
       </c>
       <c r="W80" s="8" t="n"/>
       <c r="X80" s="8" t="n"/>
-      <c r="Y80" s="8" t="n"/>
+      <c r="Y80" s="8" t="n">
+        <v>51380736</v>
+      </c>
       <c r="Z80" s="8" t="n"/>
       <c r="AA80" s="8" t="n"/>
     </row>
@@ -5655,7 +5805,9 @@
       </c>
       <c r="X81" s="8" t="n"/>
       <c r="Y81" s="8" t="n"/>
-      <c r="Z81" s="8" t="n"/>
+      <c r="Z81" s="8" t="n">
+        <v>802816</v>
+      </c>
       <c r="AA81" s="8" t="n"/>
     </row>
     <row r="82">
@@ -5718,7 +5870,9 @@
       </c>
       <c r="X82" s="8" t="n"/>
       <c r="Y82" s="8" t="n"/>
-      <c r="Z82" s="8" t="n"/>
+      <c r="Z82" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA82" s="8" t="n"/>
     </row>
     <row r="83">
@@ -5776,7 +5930,9 @@
       </c>
       <c r="Y83" s="8" t="n"/>
       <c r="Z83" s="8" t="n"/>
-      <c r="AA83" s="8" t="n"/>
+      <c r="AA83" s="8" t="n">
+        <v>401408</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="7" t="n">
@@ -5845,7 +6001,9 @@
       </c>
       <c r="W84" s="8" t="n"/>
       <c r="X84" s="8" t="n"/>
-      <c r="Y84" s="8" t="n"/>
+      <c r="Y84" s="8" t="n">
+        <v>25690368</v>
+      </c>
       <c r="Z84" s="8" t="n"/>
       <c r="AA84" s="8" t="n"/>
     </row>
@@ -5905,7 +6063,9 @@
       </c>
       <c r="X85" s="8" t="n"/>
       <c r="Y85" s="8" t="n"/>
-      <c r="Z85" s="8" t="n"/>
+      <c r="Z85" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA85" s="8" t="n"/>
     </row>
     <row r="86">
@@ -5963,7 +6123,9 @@
       </c>
       <c r="Y86" s="8" t="n"/>
       <c r="Z86" s="8" t="n"/>
-      <c r="AA86" s="8" t="n"/>
+      <c r="AA86" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="7" t="n">
@@ -6032,7 +6194,9 @@
       </c>
       <c r="W87" s="8" t="n"/>
       <c r="X87" s="8" t="n"/>
-      <c r="Y87" s="8" t="n"/>
+      <c r="Y87" s="8" t="n">
+        <v>115605760</v>
+      </c>
       <c r="Z87" s="8" t="n"/>
       <c r="AA87" s="8" t="n"/>
     </row>
@@ -6092,7 +6256,9 @@
       </c>
       <c r="X88" s="8" t="n"/>
       <c r="Y88" s="8" t="n"/>
-      <c r="Z88" s="8" t="n"/>
+      <c r="Z88" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA88" s="8" t="n"/>
     </row>
     <row r="89">
@@ -6150,7 +6316,9 @@
       </c>
       <c r="Y89" s="8" t="n"/>
       <c r="Z89" s="8" t="n"/>
-      <c r="AA89" s="8" t="n"/>
+      <c r="AA89" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="7" t="n">
@@ -6219,7 +6387,9 @@
       </c>
       <c r="W90" s="8" t="n"/>
       <c r="X90" s="8" t="n"/>
-      <c r="Y90" s="8" t="n"/>
+      <c r="Y90" s="8" t="n">
+        <v>102761472</v>
+      </c>
       <c r="Z90" s="8" t="n"/>
       <c r="AA90" s="8" t="n"/>
     </row>
@@ -6290,7 +6460,9 @@
       </c>
       <c r="W91" s="8" t="n"/>
       <c r="X91" s="8" t="n"/>
-      <c r="Y91" s="8" t="n"/>
+      <c r="Y91" s="8" t="n">
+        <v>51381248</v>
+      </c>
       <c r="Z91" s="8" t="n"/>
       <c r="AA91" s="8" t="n"/>
     </row>
@@ -6350,7 +6522,9 @@
       </c>
       <c r="X92" s="8" t="n"/>
       <c r="Y92" s="8" t="n"/>
-      <c r="Z92" s="8" t="n"/>
+      <c r="Z92" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA92" s="8" t="n"/>
     </row>
     <row r="93">
@@ -6409,7 +6583,9 @@
       </c>
       <c r="X93" s="8" t="n"/>
       <c r="Y93" s="8" t="n"/>
-      <c r="Z93" s="8" t="n"/>
+      <c r="Z93" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA93" s="8" t="n"/>
     </row>
     <row r="94">
@@ -6472,7 +6648,9 @@
       </c>
       <c r="X94" s="8" t="n"/>
       <c r="Y94" s="8" t="n"/>
-      <c r="Z94" s="8" t="n"/>
+      <c r="Z94" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA94" s="8" t="n"/>
     </row>
     <row r="95">
@@ -6530,7 +6708,9 @@
       </c>
       <c r="Y95" s="8" t="n"/>
       <c r="Z95" s="8" t="n"/>
-      <c r="AA95" s="8" t="n"/>
+      <c r="AA95" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="7" t="n">
@@ -6599,7 +6779,9 @@
       </c>
       <c r="W96" s="8" t="n"/>
       <c r="X96" s="8" t="n"/>
-      <c r="Y96" s="8" t="n"/>
+      <c r="Y96" s="8" t="n">
+        <v>51380480</v>
+      </c>
       <c r="Z96" s="8" t="n"/>
       <c r="AA96" s="8" t="n"/>
     </row>
@@ -6659,7 +6841,9 @@
       </c>
       <c r="X97" s="8" t="n"/>
       <c r="Y97" s="8" t="n"/>
-      <c r="Z97" s="8" t="n"/>
+      <c r="Z97" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA97" s="8" t="n"/>
     </row>
     <row r="98">
@@ -6717,7 +6901,9 @@
       </c>
       <c r="Y98" s="8" t="n"/>
       <c r="Z98" s="8" t="n"/>
-      <c r="AA98" s="8" t="n"/>
+      <c r="AA98" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="7" t="n">
@@ -6786,7 +6972,9 @@
       </c>
       <c r="W99" s="8" t="n"/>
       <c r="X99" s="8" t="n"/>
-      <c r="Y99" s="8" t="n"/>
+      <c r="Y99" s="8" t="n">
+        <v>115605760</v>
+      </c>
       <c r="Z99" s="8" t="n"/>
       <c r="AA99" s="8" t="n"/>
     </row>
@@ -6846,7 +7034,9 @@
       </c>
       <c r="X100" s="8" t="n"/>
       <c r="Y100" s="8" t="n"/>
-      <c r="Z100" s="8" t="n"/>
+      <c r="Z100" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA100" s="8" t="n"/>
     </row>
     <row r="101">
@@ -6904,7 +7094,9 @@
       </c>
       <c r="Y101" s="8" t="n"/>
       <c r="Z101" s="8" t="n"/>
-      <c r="AA101" s="8" t="n"/>
+      <c r="AA101" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="7" t="n">
@@ -6973,7 +7165,9 @@
       </c>
       <c r="W102" s="8" t="n"/>
       <c r="X102" s="8" t="n"/>
-      <c r="Y102" s="8" t="n"/>
+      <c r="Y102" s="8" t="n">
+        <v>51381248</v>
+      </c>
       <c r="Z102" s="8" t="n"/>
       <c r="AA102" s="8" t="n"/>
     </row>
@@ -7033,7 +7227,9 @@
       </c>
       <c r="X103" s="8" t="n"/>
       <c r="Y103" s="8" t="n"/>
-      <c r="Z103" s="8" t="n"/>
+      <c r="Z103" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA103" s="8" t="n"/>
     </row>
     <row r="104">
@@ -7096,7 +7292,9 @@
       </c>
       <c r="X104" s="8" t="n"/>
       <c r="Y104" s="8" t="n"/>
-      <c r="Z104" s="8" t="n"/>
+      <c r="Z104" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA104" s="8" t="n"/>
     </row>
     <row r="105">
@@ -7154,7 +7352,9 @@
       </c>
       <c r="Y105" s="8" t="n"/>
       <c r="Z105" s="8" t="n"/>
-      <c r="AA105" s="8" t="n"/>
+      <c r="AA105" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="7" t="n">
@@ -7223,7 +7423,9 @@
       </c>
       <c r="W106" s="8" t="n"/>
       <c r="X106" s="8" t="n"/>
-      <c r="Y106" s="8" t="n"/>
+      <c r="Y106" s="8" t="n">
+        <v>51380480</v>
+      </c>
       <c r="Z106" s="8" t="n"/>
       <c r="AA106" s="8" t="n"/>
     </row>
@@ -7283,7 +7485,9 @@
       </c>
       <c r="X107" s="8" t="n"/>
       <c r="Y107" s="8" t="n"/>
-      <c r="Z107" s="8" t="n"/>
+      <c r="Z107" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA107" s="8" t="n"/>
     </row>
     <row r="108">
@@ -7341,7 +7545,9 @@
       </c>
       <c r="Y108" s="8" t="n"/>
       <c r="Z108" s="8" t="n"/>
-      <c r="AA108" s="8" t="n"/>
+      <c r="AA108" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="7" t="n">
@@ -7410,7 +7616,9 @@
       </c>
       <c r="W109" s="8" t="n"/>
       <c r="X109" s="8" t="n"/>
-      <c r="Y109" s="8" t="n"/>
+      <c r="Y109" s="8" t="n">
+        <v>115605760</v>
+      </c>
       <c r="Z109" s="8" t="n"/>
       <c r="AA109" s="8" t="n"/>
     </row>
@@ -7470,7 +7678,9 @@
       </c>
       <c r="X110" s="8" t="n"/>
       <c r="Y110" s="8" t="n"/>
-      <c r="Z110" s="8" t="n"/>
+      <c r="Z110" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA110" s="8" t="n"/>
     </row>
     <row r="111">
@@ -7528,7 +7738,9 @@
       </c>
       <c r="Y111" s="8" t="n"/>
       <c r="Z111" s="8" t="n"/>
-      <c r="AA111" s="8" t="n"/>
+      <c r="AA111" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="7" t="n">
@@ -7597,7 +7809,9 @@
       </c>
       <c r="W112" s="8" t="n"/>
       <c r="X112" s="8" t="n"/>
-      <c r="Y112" s="8" t="n"/>
+      <c r="Y112" s="8" t="n">
+        <v>51381248</v>
+      </c>
       <c r="Z112" s="8" t="n"/>
       <c r="AA112" s="8" t="n"/>
     </row>
@@ -7657,7 +7871,9 @@
       </c>
       <c r="X113" s="8" t="n"/>
       <c r="Y113" s="8" t="n"/>
-      <c r="Z113" s="8" t="n"/>
+      <c r="Z113" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA113" s="8" t="n"/>
     </row>
     <row r="114">
@@ -7720,7 +7936,9 @@
       </c>
       <c r="X114" s="8" t="n"/>
       <c r="Y114" s="8" t="n"/>
-      <c r="Z114" s="8" t="n"/>
+      <c r="Z114" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA114" s="8" t="n"/>
     </row>
     <row r="115">
@@ -7778,7 +7996,9 @@
       </c>
       <c r="Y115" s="8" t="n"/>
       <c r="Z115" s="8" t="n"/>
-      <c r="AA115" s="8" t="n"/>
+      <c r="AA115" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="7" t="n">
@@ -7847,7 +8067,9 @@
       </c>
       <c r="W116" s="8" t="n"/>
       <c r="X116" s="8" t="n"/>
-      <c r="Y116" s="8" t="n"/>
+      <c r="Y116" s="8" t="n">
+        <v>51380480</v>
+      </c>
       <c r="Z116" s="8" t="n"/>
       <c r="AA116" s="8" t="n"/>
     </row>
@@ -7907,7 +8129,9 @@
       </c>
       <c r="X117" s="8" t="n"/>
       <c r="Y117" s="8" t="n"/>
-      <c r="Z117" s="8" t="n"/>
+      <c r="Z117" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA117" s="8" t="n"/>
     </row>
     <row r="118">
@@ -7965,7 +8189,9 @@
       </c>
       <c r="Y118" s="8" t="n"/>
       <c r="Z118" s="8" t="n"/>
-      <c r="AA118" s="8" t="n"/>
+      <c r="AA118" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="7" t="n">
@@ -8034,7 +8260,9 @@
       </c>
       <c r="W119" s="8" t="n"/>
       <c r="X119" s="8" t="n"/>
-      <c r="Y119" s="8" t="n"/>
+      <c r="Y119" s="8" t="n">
+        <v>115605760</v>
+      </c>
       <c r="Z119" s="8" t="n"/>
       <c r="AA119" s="8" t="n"/>
     </row>
@@ -8094,7 +8322,9 @@
       </c>
       <c r="X120" s="8" t="n"/>
       <c r="Y120" s="8" t="n"/>
-      <c r="Z120" s="8" t="n"/>
+      <c r="Z120" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA120" s="8" t="n"/>
     </row>
     <row r="121">
@@ -8152,7 +8382,9 @@
       </c>
       <c r="Y121" s="8" t="n"/>
       <c r="Z121" s="8" t="n"/>
-      <c r="AA121" s="8" t="n"/>
+      <c r="AA121" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="7" t="n">
@@ -8221,7 +8453,9 @@
       </c>
       <c r="W122" s="8" t="n"/>
       <c r="X122" s="8" t="n"/>
-      <c r="Y122" s="8" t="n"/>
+      <c r="Y122" s="8" t="n">
+        <v>51381248</v>
+      </c>
       <c r="Z122" s="8" t="n"/>
       <c r="AA122" s="8" t="n"/>
     </row>
@@ -8281,7 +8515,9 @@
       </c>
       <c r="X123" s="8" t="n"/>
       <c r="Y123" s="8" t="n"/>
-      <c r="Z123" s="8" t="n"/>
+      <c r="Z123" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA123" s="8" t="n"/>
     </row>
     <row r="124">
@@ -8344,7 +8580,9 @@
       </c>
       <c r="X124" s="8" t="n"/>
       <c r="Y124" s="8" t="n"/>
-      <c r="Z124" s="8" t="n"/>
+      <c r="Z124" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA124" s="8" t="n"/>
     </row>
     <row r="125">
@@ -8402,7 +8640,9 @@
       </c>
       <c r="Y125" s="8" t="n"/>
       <c r="Z125" s="8" t="n"/>
-      <c r="AA125" s="8" t="n"/>
+      <c r="AA125" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="7" t="n">
@@ -8471,7 +8711,9 @@
       </c>
       <c r="W126" s="8" t="n"/>
       <c r="X126" s="8" t="n"/>
-      <c r="Y126" s="8" t="n"/>
+      <c r="Y126" s="8" t="n">
+        <v>51380480</v>
+      </c>
       <c r="Z126" s="8" t="n"/>
       <c r="AA126" s="8" t="n"/>
     </row>
@@ -8531,7 +8773,9 @@
       </c>
       <c r="X127" s="8" t="n"/>
       <c r="Y127" s="8" t="n"/>
-      <c r="Z127" s="8" t="n"/>
+      <c r="Z127" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA127" s="8" t="n"/>
     </row>
     <row r="128">
@@ -8589,7 +8833,9 @@
       </c>
       <c r="Y128" s="8" t="n"/>
       <c r="Z128" s="8" t="n"/>
-      <c r="AA128" s="8" t="n"/>
+      <c r="AA128" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="7" t="n">
@@ -8658,7 +8904,9 @@
       </c>
       <c r="W129" s="8" t="n"/>
       <c r="X129" s="8" t="n"/>
-      <c r="Y129" s="8" t="n"/>
+      <c r="Y129" s="8" t="n">
+        <v>115605760</v>
+      </c>
       <c r="Z129" s="8" t="n"/>
       <c r="AA129" s="8" t="n"/>
     </row>
@@ -8718,7 +8966,9 @@
       </c>
       <c r="X130" s="8" t="n"/>
       <c r="Y130" s="8" t="n"/>
-      <c r="Z130" s="8" t="n"/>
+      <c r="Z130" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA130" s="8" t="n"/>
     </row>
     <row r="131">
@@ -8776,7 +9026,9 @@
       </c>
       <c r="Y131" s="8" t="n"/>
       <c r="Z131" s="8" t="n"/>
-      <c r="AA131" s="8" t="n"/>
+      <c r="AA131" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="7" t="n">
@@ -8845,7 +9097,9 @@
       </c>
       <c r="W132" s="8" t="n"/>
       <c r="X132" s="8" t="n"/>
-      <c r="Y132" s="8" t="n"/>
+      <c r="Y132" s="8" t="n">
+        <v>51381248</v>
+      </c>
       <c r="Z132" s="8" t="n"/>
       <c r="AA132" s="8" t="n"/>
     </row>
@@ -8905,7 +9159,9 @@
       </c>
       <c r="X133" s="8" t="n"/>
       <c r="Y133" s="8" t="n"/>
-      <c r="Z133" s="8" t="n"/>
+      <c r="Z133" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA133" s="8" t="n"/>
     </row>
     <row r="134">
@@ -8968,7 +9224,9 @@
       </c>
       <c r="X134" s="8" t="n"/>
       <c r="Y134" s="8" t="n"/>
-      <c r="Z134" s="8" t="n"/>
+      <c r="Z134" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA134" s="8" t="n"/>
     </row>
     <row r="135">
@@ -9026,7 +9284,9 @@
       </c>
       <c r="Y135" s="8" t="n"/>
       <c r="Z135" s="8" t="n"/>
-      <c r="AA135" s="8" t="n"/>
+      <c r="AA135" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="7" t="n">
@@ -9095,7 +9355,9 @@
       </c>
       <c r="W136" s="8" t="n"/>
       <c r="X136" s="8" t="n"/>
-      <c r="Y136" s="8" t="n"/>
+      <c r="Y136" s="8" t="n">
+        <v>51380480</v>
+      </c>
       <c r="Z136" s="8" t="n"/>
       <c r="AA136" s="8" t="n"/>
     </row>
@@ -9155,7 +9417,9 @@
       </c>
       <c r="X137" s="8" t="n"/>
       <c r="Y137" s="8" t="n"/>
-      <c r="Z137" s="8" t="n"/>
+      <c r="Z137" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA137" s="8" t="n"/>
     </row>
     <row r="138">
@@ -9213,7 +9477,9 @@
       </c>
       <c r="Y138" s="8" t="n"/>
       <c r="Z138" s="8" t="n"/>
-      <c r="AA138" s="8" t="n"/>
+      <c r="AA138" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="n">
@@ -9282,7 +9548,9 @@
       </c>
       <c r="W139" s="8" t="n"/>
       <c r="X139" s="8" t="n"/>
-      <c r="Y139" s="8" t="n"/>
+      <c r="Y139" s="8" t="n">
+        <v>115605760</v>
+      </c>
       <c r="Z139" s="8" t="n"/>
       <c r="AA139" s="8" t="n"/>
     </row>
@@ -9342,7 +9610,9 @@
       </c>
       <c r="X140" s="8" t="n"/>
       <c r="Y140" s="8" t="n"/>
-      <c r="Z140" s="8" t="n"/>
+      <c r="Z140" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA140" s="8" t="n"/>
     </row>
     <row r="141">
@@ -9400,7 +9670,9 @@
       </c>
       <c r="Y141" s="8" t="n"/>
       <c r="Z141" s="8" t="n"/>
-      <c r="AA141" s="8" t="n"/>
+      <c r="AA141" s="8" t="n">
+        <v>50176</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="7" t="n">
@@ -9469,7 +9741,9 @@
       </c>
       <c r="W142" s="8" t="n"/>
       <c r="X142" s="8" t="n"/>
-      <c r="Y142" s="8" t="n"/>
+      <c r="Y142" s="8" t="n">
+        <v>51381248</v>
+      </c>
       <c r="Z142" s="8" t="n"/>
       <c r="AA142" s="8" t="n"/>
     </row>
@@ -9529,7 +9803,9 @@
       </c>
       <c r="X143" s="8" t="n"/>
       <c r="Y143" s="8" t="n"/>
-      <c r="Z143" s="8" t="n"/>
+      <c r="Z143" s="8" t="n">
+        <v>401408</v>
+      </c>
       <c r="AA143" s="8" t="n"/>
     </row>
     <row r="144">
@@ -9592,7 +9868,9 @@
       </c>
       <c r="X144" s="8" t="n"/>
       <c r="Y144" s="8" t="n"/>
-      <c r="Z144" s="8" t="n"/>
+      <c r="Z144" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA144" s="8" t="n"/>
     </row>
     <row r="145">
@@ -9650,7 +9928,9 @@
       </c>
       <c r="Y145" s="8" t="n"/>
       <c r="Z145" s="8" t="n"/>
-      <c r="AA145" s="8" t="n"/>
+      <c r="AA145" s="8" t="n">
+        <v>200704</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="7" t="n">
@@ -9719,7 +9999,9 @@
       </c>
       <c r="W146" s="8" t="n"/>
       <c r="X146" s="8" t="n"/>
-      <c r="Y146" s="8" t="n"/>
+      <c r="Y146" s="8" t="n">
+        <v>25690624</v>
+      </c>
       <c r="Z146" s="8" t="n"/>
       <c r="AA146" s="8" t="n"/>
     </row>
@@ -9779,7 +10061,9 @@
       </c>
       <c r="X147" s="8" t="n"/>
       <c r="Y147" s="8" t="n"/>
-      <c r="Z147" s="8" t="n"/>
+      <c r="Z147" s="8" t="n">
+        <v>50176</v>
+      </c>
       <c r="AA147" s="8" t="n"/>
     </row>
     <row r="148">
@@ -9837,7 +10121,9 @@
       </c>
       <c r="Y148" s="8" t="n"/>
       <c r="Z148" s="8" t="n"/>
-      <c r="AA148" s="8" t="n"/>
+      <c r="AA148" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="7" t="n">
@@ -9906,7 +10192,9 @@
       </c>
       <c r="W149" s="8" t="n"/>
       <c r="X149" s="8" t="n"/>
-      <c r="Y149" s="8" t="n"/>
+      <c r="Y149" s="8" t="n">
+        <v>115606016</v>
+      </c>
       <c r="Z149" s="8" t="n"/>
       <c r="AA149" s="8" t="n"/>
     </row>
@@ -9966,7 +10254,9 @@
       </c>
       <c r="X150" s="8" t="n"/>
       <c r="Y150" s="8" t="n"/>
-      <c r="Z150" s="8" t="n"/>
+      <c r="Z150" s="8" t="n">
+        <v>50176</v>
+      </c>
       <c r="AA150" s="8" t="n"/>
     </row>
     <row r="151">
@@ -10024,7 +10314,9 @@
       </c>
       <c r="Y151" s="8" t="n"/>
       <c r="Z151" s="8" t="n"/>
-      <c r="AA151" s="8" t="n"/>
+      <c r="AA151" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="7" t="n">
@@ -10093,7 +10385,9 @@
       </c>
       <c r="W152" s="8" t="n"/>
       <c r="X152" s="8" t="n"/>
-      <c r="Y152" s="8" t="n"/>
+      <c r="Y152" s="8" t="n">
+        <v>102762496</v>
+      </c>
       <c r="Z152" s="8" t="n"/>
       <c r="AA152" s="8" t="n"/>
     </row>
@@ -10164,7 +10458,9 @@
       </c>
       <c r="W153" s="8" t="n"/>
       <c r="X153" s="8" t="n"/>
-      <c r="Y153" s="8" t="n"/>
+      <c r="Y153" s="8" t="n">
+        <v>51382272</v>
+      </c>
       <c r="Z153" s="8" t="n"/>
       <c r="AA153" s="8" t="n"/>
     </row>
@@ -10224,7 +10520,9 @@
       </c>
       <c r="X154" s="8" t="n"/>
       <c r="Y154" s="8" t="n"/>
-      <c r="Z154" s="8" t="n"/>
+      <c r="Z154" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA154" s="8" t="n"/>
     </row>
     <row r="155">
@@ -10283,7 +10581,9 @@
       </c>
       <c r="X155" s="8" t="n"/>
       <c r="Y155" s="8" t="n"/>
-      <c r="Z155" s="8" t="n"/>
+      <c r="Z155" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA155" s="8" t="n"/>
     </row>
     <row r="156">
@@ -10346,7 +10646,9 @@
       </c>
       <c r="X156" s="8" t="n"/>
       <c r="Y156" s="8" t="n"/>
-      <c r="Z156" s="8" t="n"/>
+      <c r="Z156" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA156" s="8" t="n"/>
     </row>
     <row r="157">
@@ -10404,7 +10706,9 @@
       </c>
       <c r="Y157" s="8" t="n"/>
       <c r="Z157" s="8" t="n"/>
-      <c r="AA157" s="8" t="n"/>
+      <c r="AA157" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="7" t="n">
@@ -10473,7 +10777,9 @@
       </c>
       <c r="W158" s="8" t="n"/>
       <c r="X158" s="8" t="n"/>
-      <c r="Y158" s="8" t="n"/>
+      <c r="Y158" s="8" t="n">
+        <v>51380736</v>
+      </c>
       <c r="Z158" s="8" t="n"/>
       <c r="AA158" s="8" t="n"/>
     </row>
@@ -10533,7 +10839,9 @@
       </c>
       <c r="X159" s="8" t="n"/>
       <c r="Y159" s="8" t="n"/>
-      <c r="Z159" s="8" t="n"/>
+      <c r="Z159" s="8" t="n">
+        <v>50176</v>
+      </c>
       <c r="AA159" s="8" t="n"/>
     </row>
     <row r="160">
@@ -10591,7 +10899,9 @@
       </c>
       <c r="Y160" s="8" t="n"/>
       <c r="Z160" s="8" t="n"/>
-      <c r="AA160" s="8" t="n"/>
+      <c r="AA160" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="7" t="n">
@@ -10660,7 +10970,9 @@
       </c>
       <c r="W161" s="8" t="n"/>
       <c r="X161" s="8" t="n"/>
-      <c r="Y161" s="8" t="n"/>
+      <c r="Y161" s="8" t="n">
+        <v>115606016</v>
+      </c>
       <c r="Z161" s="8" t="n"/>
       <c r="AA161" s="8" t="n"/>
     </row>
@@ -10720,7 +11032,9 @@
       </c>
       <c r="X162" s="8" t="n"/>
       <c r="Y162" s="8" t="n"/>
-      <c r="Z162" s="8" t="n"/>
+      <c r="Z162" s="8" t="n">
+        <v>50176</v>
+      </c>
       <c r="AA162" s="8" t="n"/>
     </row>
     <row r="163">
@@ -10778,7 +11092,9 @@
       </c>
       <c r="Y163" s="8" t="n"/>
       <c r="Z163" s="8" t="n"/>
-      <c r="AA163" s="8" t="n"/>
+      <c r="AA163" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="7" t="n">
@@ -10847,7 +11163,9 @@
       </c>
       <c r="W164" s="8" t="n"/>
       <c r="X164" s="8" t="n"/>
-      <c r="Y164" s="8" t="n"/>
+      <c r="Y164" s="8" t="n">
+        <v>51382272</v>
+      </c>
       <c r="Z164" s="8" t="n"/>
       <c r="AA164" s="8" t="n"/>
     </row>
@@ -10907,7 +11225,9 @@
       </c>
       <c r="X165" s="8" t="n"/>
       <c r="Y165" s="8" t="n"/>
-      <c r="Z165" s="8" t="n"/>
+      <c r="Z165" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA165" s="8" t="n"/>
     </row>
     <row r="166">
@@ -10970,7 +11290,9 @@
       </c>
       <c r="X166" s="8" t="n"/>
       <c r="Y166" s="8" t="n"/>
-      <c r="Z166" s="8" t="n"/>
+      <c r="Z166" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA166" s="8" t="n"/>
     </row>
     <row r="167">
@@ -11028,7 +11350,9 @@
       </c>
       <c r="Y167" s="8" t="n"/>
       <c r="Z167" s="8" t="n"/>
-      <c r="AA167" s="8" t="n"/>
+      <c r="AA167" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="7" t="n">
@@ -11097,7 +11421,9 @@
       </c>
       <c r="W168" s="8" t="n"/>
       <c r="X168" s="8" t="n"/>
-      <c r="Y168" s="8" t="n"/>
+      <c r="Y168" s="8" t="n">
+        <v>51380736</v>
+      </c>
       <c r="Z168" s="8" t="n"/>
       <c r="AA168" s="8" t="n"/>
     </row>
@@ -11157,7 +11483,9 @@
       </c>
       <c r="X169" s="8" t="n"/>
       <c r="Y169" s="8" t="n"/>
-      <c r="Z169" s="8" t="n"/>
+      <c r="Z169" s="8" t="n">
+        <v>50176</v>
+      </c>
       <c r="AA169" s="8" t="n"/>
     </row>
     <row r="170">
@@ -11215,7 +11543,9 @@
       </c>
       <c r="Y170" s="8" t="n"/>
       <c r="Z170" s="8" t="n"/>
-      <c r="AA170" s="8" t="n"/>
+      <c r="AA170" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="7" t="n">
@@ -11284,7 +11614,9 @@
       </c>
       <c r="W171" s="8" t="n"/>
       <c r="X171" s="8" t="n"/>
-      <c r="Y171" s="8" t="n"/>
+      <c r="Y171" s="8" t="n">
+        <v>115606016</v>
+      </c>
       <c r="Z171" s="8" t="n"/>
       <c r="AA171" s="8" t="n"/>
     </row>
@@ -11344,7 +11676,9 @@
       </c>
       <c r="X172" s="8" t="n"/>
       <c r="Y172" s="8" t="n"/>
-      <c r="Z172" s="8" t="n"/>
+      <c r="Z172" s="8" t="n">
+        <v>50176</v>
+      </c>
       <c r="AA172" s="8" t="n"/>
     </row>
     <row r="173">
@@ -11402,7 +11736,9 @@
       </c>
       <c r="Y173" s="8" t="n"/>
       <c r="Z173" s="8" t="n"/>
-      <c r="AA173" s="8" t="n"/>
+      <c r="AA173" s="8" t="n">
+        <v>25088</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="7" t="n">
@@ -11471,7 +11807,9 @@
       </c>
       <c r="W174" s="8" t="n"/>
       <c r="X174" s="8" t="n"/>
-      <c r="Y174" s="8" t="n"/>
+      <c r="Y174" s="8" t="n">
+        <v>51382272</v>
+      </c>
       <c r="Z174" s="8" t="n"/>
       <c r="AA174" s="8" t="n"/>
     </row>
@@ -11531,7 +11869,9 @@
       </c>
       <c r="X175" s="8" t="n"/>
       <c r="Y175" s="8" t="n"/>
-      <c r="Z175" s="8" t="n"/>
+      <c r="Z175" s="8" t="n">
+        <v>200704</v>
+      </c>
       <c r="AA175" s="8" t="n"/>
     </row>
     <row r="176">
@@ -11594,7 +11934,9 @@
       </c>
       <c r="X176" s="8" t="n"/>
       <c r="Y176" s="8" t="n"/>
-      <c r="Z176" s="8" t="n"/>
+      <c r="Z176" s="8" t="n">
+        <v>100352</v>
+      </c>
       <c r="AA176" s="8" t="n"/>
     </row>
     <row r="177">
@@ -11652,7 +11994,9 @@
       </c>
       <c r="Y177" s="8" t="n"/>
       <c r="Z177" s="8" t="n"/>
-      <c r="AA177" s="8" t="n"/>
+      <c r="AA177" s="8" t="n">
+        <v>100352</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="7" t="n">
@@ -11704,7 +12048,9 @@
       </c>
       <c r="X178" s="8" t="n"/>
       <c r="Y178" s="8" t="n"/>
-      <c r="Z178" s="8" t="n"/>
+      <c r="Z178" s="8" t="n">
+        <v>98304</v>
+      </c>
       <c r="AA178" s="8" t="n"/>
     </row>
     <row r="179">
@@ -11756,9 +12102,13 @@
       <c r="X179" s="8" t="n">
         <v>2048</v>
       </c>
-      <c r="Y179" s="8" t="n"/>
+      <c r="Y179" s="8" t="n">
+        <v>2049000</v>
+      </c>
       <c r="Z179" s="8" t="n"/>
-      <c r="AA179" s="8" t="n"/>
+      <c r="AA179" s="8" t="n">
+        <v>2048</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -11790,7 +12140,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="Y1:Y179">
     <cfRule type="cellIs" priority="4" operator="equal" dxfId="3" stopIfTrue="1">
-      <formula>0</formula>
+      <formula>118014016</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11859,7 +12209,7 @@
         </is>
       </c>
       <c r="B5" s="8" t="n">
-        <v>0</v>
+        <v>3.858000808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>